<commit_message>
chore: update input file of TDD case1 to last version
Updated input files used to run the test case 1 for the TDD to the last version already available in folder ..\source_code\input_files\input_file_template.

modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_1_coupling.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_1_input.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_1_operation.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_definition.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_diagnostic.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/conductor_grid.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/environment_input.xlsx
modified:   ../TDD_examples/CASE_1_ITER_like_LTS/transitory_input.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_1_ITER_like_LTS/conductor_1_coupling.xlsx
+++ b/TDD_examples/CASE_1_ITER_like_LTS/conductor_1_coupling.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/SC2_38/Description_of_Components/ITER_TF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_1_ITER_like_LTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{76561CA3-E0AF-4EC9-BADE-7B4233765AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F29148B9-F144-440B-927D-9957801C4469}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5432281-88FA-4928-A5C2-9B59082EB736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3270" yWindow="1210" windowWidth="14400" windowHeight="7360" tabRatio="663" firstSheet="1" activeTab="3" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="663" xr2:uid="{91AAA46A-E77A-4CF9-A2A6-D526EB86D7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_perimeter_flag" sheetId="8" r:id="rId1"/>
     <sheet name="contact_perimeter" sheetId="1" r:id="rId2"/>
     <sheet name="HTC_choice" sheetId="4" r:id="rId3"/>
     <sheet name="contact_HTC" sheetId="2" r:id="rId4"/>
-    <sheet name="HTC_multiplier" sheetId="5" r:id="rId5"/>
-    <sheet name="open_perimeter_fract" sheetId="3" r:id="rId6"/>
-    <sheet name="interf_thickness" sheetId="7" r:id="rId7"/>
-    <sheet name="trans_transp_multiplier" sheetId="6" r:id="rId8"/>
-    <sheet name="view_factors" sheetId="9" r:id="rId9"/>
+    <sheet name="thermal_contact_resistance" sheetId="10" r:id="rId5"/>
+    <sheet name="HTC_multiplier" sheetId="5" r:id="rId6"/>
+    <sheet name="electric_conductance_mode" sheetId="11" r:id="rId7"/>
+    <sheet name="electric_conductance" sheetId="12" r:id="rId8"/>
+    <sheet name="open_perimeter_fract" sheetId="3" r:id="rId9"/>
+    <sheet name="interf_thickness" sheetId="7" r:id="rId10"/>
+    <sheet name="trans_transp_multiplier" sheetId="6" r:id="rId11"/>
+    <sheet name="view_factors" sheetId="9" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>[%] Fraction of the contact perimeter between fluid elements which is actually open</t>
   </si>
@@ -74,6 +77,15 @@
   </si>
   <si>
     <t>Environment</t>
+  </si>
+  <si>
+    <t>[m2K/W] thermal contact resistance between soldi component, should be &gt;= 0; used if flag HTC_choice is 1</t>
+  </si>
+  <si>
+    <t>Flag to specify the kind of electric conductance: 1 conductance per unit length (the contact is along a line as for tow cilinder); 2 = actual conductance between components.</t>
+  </si>
+  <si>
+    <t>[S/m] Value of the electric_conductance</t>
   </si>
 </sst>
 </file>
@@ -143,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -154,14 +166,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
@@ -174,13 +180,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -604,8 +606,8 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="CHAN"/>
+      <sheetName val="STACK"/>
       <sheetName val="STR_MIX"/>
-      <sheetName val="STR_SC"/>
       <sheetName val="STR_STAB"/>
       <sheetName val="Z_JACKET"/>
     </sheetNames>
@@ -620,14 +622,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
         <row r="3">
           <cell r="E3" t="str">
             <v>STR_MIX_1</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="3">
@@ -940,94 +942,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631F8432-32B0-4782-8A41-3C8B7D94A95A}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:AB1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>[1]CHAN!$E$3</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>[1]CHAN!F$3</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>[1]STR_MIX!$E$3</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>[1]Z_JACKET!$E$3</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1036,19 +1038,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1060,16 +1062,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1102,6 +1104,535 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182F8F7F-A8D7-4239-AF85-1CCD06F5862A}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{11073E0C-B0B4-4CCC-ADAF-F7C7AD75C766}">
+            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{D8D42210-C82D-40ED-B579-6A74980D2860}">
+            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF3B1F8-15BE-471B-8C90-C91254905B72}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{375370F1-6A9D-44F9-97E7-5F19EF16D901}">
+            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{D8851FDB-4F41-4BDA-A3BC-4D0318F65BF8}">
+            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF92D050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C628F5-9BDA-4746-9BD5-872CA60F8FA3}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE57BE0-CB95-4186-8582-DA069D805E4E}">
   <dimension ref="A1:F7"/>
@@ -1110,91 +1641,91 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="str">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.13569999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f>0.009*PI()</f>
         <v>2.8274333882308135E-2</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1203,21 +1734,21 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f>3.7275</f>
         <v>3.7275</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f>0.094356</f>
         <v>9.4355999999999995E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1229,17 +1760,17 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f>0.031452</f>
         <v>3.1452000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1416,118 +1947,118 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="103.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:6" ht="103.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
         <f>-2</f>
         <v>-2</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
         <f>-2</f>
         <v>-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f>-2</f>
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1536,19 +2067,19 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -1562,7 +2093,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1724,95 +2255,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A5B995-3590-4E28-8701-A823419A209A}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1000</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -1821,19 +2352,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -1845,16 +2376,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -2021,6 +2552,160 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84979D30-2F55-48C2-BE9B-5BE9A7CD8793}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF123C-7F60-4807-AE29-ECD4FCE24EA7}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2028,91 +2713,91 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -2121,19 +2806,19 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -2145,16 +2830,16 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -2320,7 +3005,314 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE093F0-40AE-4717-81EF-811E4283AACB}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB08AF8-C0A1-4C4B-9882-4C8E380BC3C6}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="str">
+        <f>contact_perimeter_flag!B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>contact_perimeter_flag!C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>contact_perimeter_flag!D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>contact_perimeter_flag!E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f>contact_perimeter_flag!F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f>B2</f>
+        <v>Environment</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f>C2</f>
+        <v>CHAN_1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f>D2</f>
+        <v>CHAN_2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f>E2</f>
+        <v>STR_MIX_1</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f>F2</f>
+        <v>Z_JACKET_1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B35E1EA-762F-42F4-ACD0-F98E1885F191}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2328,77 +3320,77 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
+      <c r="B2" s="4" t="str">
         <f>contact_perimeter_flag!B2</f>
         <v>Environment</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C2" s="4" t="str">
         <f>contact_perimeter_flag!C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="D2" s="5" t="str">
+      <c r="D2" s="4" t="str">
         <f>contact_perimeter_flag!D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="E2" s="5" t="str">
+      <c r="E2" s="4" t="str">
         <f>contact_perimeter_flag!E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="4" t="str">
         <f>contact_perimeter_flag!F2</f>
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
         <f>B2</f>
         <v>Environment</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
         <f>C2</f>
         <v>CHAN_1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>0.293</f>
         <v>0.29299999999999998</v>
       </c>
@@ -2409,18 +3401,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
         <f>D2</f>
         <v>CHAN_2</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="1">
@@ -2430,12 +3422,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
         <f>E2</f>
         <v>STR_MIX_1</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
@@ -2451,12 +3443,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
         <f>F2</f>
         <v>Z_JACKET_1</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -2507,533 +3499,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182F8F7F-A8D7-4239-AF85-1CCD06F5862A}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD57"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
-        <f>contact_perimeter_flag!B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="C2" s="5" t="str">
-        <f>contact_perimeter_flag!C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="D2" s="5" t="str">
-        <f>contact_perimeter_flag!D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="E2" s="5" t="str">
-        <f>contact_perimeter_flag!E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="F2" s="5" t="str">
-        <f>contact_perimeter_flag!F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
-        <f>B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
-        <f>C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1E-3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
-        <f>D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
-        <f>E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
-        <f>F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{11073E0C-B0B4-4CCC-ADAF-F7C7AD75C766}">
-            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{D8D42210-C82D-40ED-B579-6A74980D2860}">
-            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D4</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF3B1F8-15BE-471B-8C90-C91254905B72}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD109"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="str">
-        <f>contact_perimeter_flag!B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="C2" s="5" t="str">
-        <f>contact_perimeter_flag!C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="D2" s="5" t="str">
-        <f>contact_perimeter_flag!D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="E2" s="5" t="str">
-        <f>contact_perimeter_flag!E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="F2" s="5" t="str">
-        <f>contact_perimeter_flag!F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="str">
-        <f>B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="str">
-        <f>C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="str">
-        <f>D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="str">
-        <f>E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="B6" s="12">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="str">
-        <f>F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-      <c r="B7" s="12">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{375370F1-6A9D-44F9-97E7-5F19EF16D901}">
-            <xm:f>contact_perimeter_flag!$D$4=0</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{D8851FDB-4F41-4BDA-A3BC-4D0318F65BF8}">
-            <xm:f>contact_perimeter_flag!$D$4=1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D4</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C628F5-9BDA-4746-9BD5-872CA60F8FA3}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="str">
-        <f>contact_perimeter_flag!B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="C2" s="14" t="str">
-        <f>contact_perimeter_flag!C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="D2" s="14" t="str">
-        <f>contact_perimeter_flag!D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="E2" s="14" t="str">
-        <f>contact_perimeter_flag!E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="F2" s="14" t="str">
-        <f>contact_perimeter_flag!F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="str">
-        <f>B2</f>
-        <v>Environment</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="str">
-        <f>C2</f>
-        <v>CHAN_1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="str">
-        <f>D2</f>
-        <v>CHAN_2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="str">
-        <f>E2</f>
-        <v>STR_MIX_1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="str">
-        <f>F2</f>
-        <v>Z_JACKET_1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>